<commit_message>
added TotVetPop to zip, tract level datasets
</commit_message>
<xml_diff>
--- a/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
+++ b/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\data_final\consolidated\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CFDB40-9A4B-4493-9CA5-1A03ABED3758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E495AB0-6C07-4EE0-8E4C-FE5B34A23C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="11686" windowHeight="14483" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tractsDataDictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="368">
   <si>
     <t>Theme</t>
   </si>
@@ -1131,6 +1131,12 @@
   </si>
   <si>
     <t>494 na values</t>
+  </si>
+  <si>
+    <t>TotVetPop</t>
+  </si>
+  <si>
+    <t>Total veteran population</t>
   </si>
 </sst>
 </file>
@@ -1982,10 +1988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q128"/>
+  <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2243,22 +2249,19 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="F8" s="1" t="s">
         <v>314</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>27</v>
+        <v>366</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>28</v>
+        <v>367</v>
       </c>
       <c r="K8" s="1">
         <v>2018</v>
@@ -2267,31 +2270,20 @@
         <v>24</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>289</v>
       </c>
       <c r="O8" s="1">
-        <v>9670</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>314</v>
-      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
         <v>314</v>
       </c>
@@ -2299,10 +2291,10 @@
         <v>314</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>266</v>
+        <v>28</v>
       </c>
       <c r="K9" s="1">
         <v>2018</v>
@@ -2311,13 +2303,13 @@
         <v>24</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>289</v>
       </c>
       <c r="O9" s="1">
-        <v>4532</v>
+        <v>9670</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>322</v>
@@ -2327,15 +2319,26 @@
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>314</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>32</v>
+        <v>266</v>
       </c>
       <c r="K10" s="1">
         <v>2018</v>
@@ -2344,45 +2347,31 @@
         <v>24</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>289</v>
       </c>
       <c r="O10" s="1">
-        <v>5556</v>
+        <v>4532</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>314</v>
-      </c>
+      <c r="D11" s="3"/>
       <c r="F11" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K11" s="1">
         <v>2018</v>
@@ -2391,16 +2380,16 @@
         <v>24</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O11" s="1">
-        <v>80.290000000000006</v>
+        <v>5556</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.5">
@@ -2426,10 +2415,10 @@
         <v>314</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K12" s="1">
         <v>2018</v>
@@ -2444,7 +2433,7 @@
         <v>290</v>
       </c>
       <c r="O12" s="1">
-        <v>13.78</v>
+        <v>80.290000000000006</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>324</v>
@@ -2473,10 +2462,10 @@
         <v>314</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K13" s="1">
         <v>2018</v>
@@ -2491,7 +2480,7 @@
         <v>290</v>
       </c>
       <c r="O13" s="1">
-        <v>0</v>
+        <v>13.78</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>324</v>
@@ -2520,10 +2509,10 @@
         <v>314</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K14" s="1">
         <v>2018</v>
@@ -2538,7 +2527,7 @@
         <v>290</v>
       </c>
       <c r="O14" s="1">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>324</v>
@@ -2567,10 +2556,10 @@
         <v>314</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K15" s="1">
         <v>2018</v>
@@ -2585,7 +2574,7 @@
         <v>290</v>
       </c>
       <c r="O15" s="1">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>324</v>
@@ -2614,10 +2603,10 @@
         <v>314</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K16" s="1">
         <v>2018</v>
@@ -2632,7 +2621,7 @@
         <v>290</v>
       </c>
       <c r="O16" s="1">
-        <v>5.55</v>
+        <v>0</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>324</v>
@@ -2661,10 +2650,10 @@
         <v>314</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K17" s="1">
         <v>2018</v>
@@ -2679,7 +2668,7 @@
         <v>290</v>
       </c>
       <c r="O17" s="1">
-        <v>8.18</v>
+        <v>5.55</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>324</v>
@@ -2689,7 +2678,18 @@
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="B18" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>314</v>
       </c>
@@ -2697,10 +2697,10 @@
         <v>314</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>270</v>
+        <v>46</v>
       </c>
       <c r="K18" s="1">
         <v>2018</v>
@@ -2715,7 +2715,7 @@
         <v>290</v>
       </c>
       <c r="O18" s="1">
-        <v>0.23</v>
+        <v>8.18</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>324</v>
@@ -2725,18 +2725,7 @@
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>314</v>
-      </c>
+      <c r="D19" s="3"/>
       <c r="F19" s="1" t="s">
         <v>314</v>
       </c>
@@ -2744,10 +2733,10 @@
         <v>314</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>49</v>
+        <v>270</v>
       </c>
       <c r="K19" s="1">
         <v>2018</v>
@@ -2762,7 +2751,7 @@
         <v>290</v>
       </c>
       <c r="O19" s="1">
-        <v>14.63</v>
+        <v>0.23</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>324</v>
@@ -2787,11 +2776,14 @@
       <c r="F20" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K20" s="1">
         <v>2018</v>
@@ -2806,7 +2798,7 @@
         <v>290</v>
       </c>
       <c r="O20" s="1">
-        <v>66.83</v>
+        <v>14.63</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>324</v>
@@ -2832,10 +2824,10 @@
         <v>314</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K21" s="1">
         <v>2018</v>
@@ -2850,7 +2842,7 @@
         <v>290</v>
       </c>
       <c r="O21" s="1">
-        <v>11.45</v>
+        <v>66.83</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>324</v>
@@ -2876,10 +2868,10 @@
         <v>314</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K22" s="1">
         <v>2018</v>
@@ -2891,13 +2883,13 @@
         <v>25</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O22" s="1">
-        <v>607</v>
+        <v>11.45</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.5">
@@ -2920,10 +2912,10 @@
         <v>314</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K23" s="1">
         <v>2018</v>
@@ -2938,7 +2930,7 @@
         <v>289</v>
       </c>
       <c r="O23" s="1">
-        <v>1070</v>
+        <v>607</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>322</v>
@@ -2964,10 +2956,10 @@
         <v>314</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K24" s="1">
         <v>2018</v>
@@ -2982,7 +2974,7 @@
         <v>289</v>
       </c>
       <c r="O24" s="1">
-        <v>722</v>
+        <v>1070</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>322</v>
@@ -3008,10 +3000,10 @@
         <v>314</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K25" s="1">
         <v>2018</v>
@@ -3026,7 +3018,7 @@
         <v>289</v>
       </c>
       <c r="O25" s="1">
-        <v>704</v>
+        <v>722</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>322</v>
@@ -3052,10 +3044,10 @@
         <v>314</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K26" s="1">
         <v>2018</v>
@@ -3070,7 +3062,7 @@
         <v>289</v>
       </c>
       <c r="O26" s="1">
-        <v>4835</v>
+        <v>704</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>322</v>
@@ -3080,6 +3072,9 @@
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B27" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>314</v>
       </c>
@@ -3093,10 +3088,10 @@
         <v>314</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K27" s="1">
         <v>2018</v>
@@ -3111,7 +3106,7 @@
         <v>289</v>
       </c>
       <c r="O27" s="1">
-        <v>495</v>
+        <v>4835</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>322</v>
@@ -3134,10 +3129,10 @@
         <v>314</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K28" s="1">
         <v>2018</v>
@@ -3152,7 +3147,7 @@
         <v>289</v>
       </c>
       <c r="O28" s="1">
-        <v>531</v>
+        <v>495</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>322</v>
@@ -3162,9 +3157,6 @@
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="C29" s="1" t="s">
         <v>314</v>
       </c>
@@ -3178,10 +3170,10 @@
         <v>314</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K29" s="1">
         <v>2018</v>
@@ -3196,7 +3188,7 @@
         <v>289</v>
       </c>
       <c r="O29" s="1">
-        <v>718</v>
+        <v>531</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>322</v>
@@ -3222,10 +3214,10 @@
         <v>314</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K30" s="1">
         <v>2018</v>
@@ -3240,7 +3232,7 @@
         <v>289</v>
       </c>
       <c r="O30" s="1">
-        <v>372</v>
+        <v>718</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>322</v>
@@ -3266,10 +3258,10 @@
         <v>314</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K31" s="1">
         <v>2018</v>
@@ -3284,7 +3276,7 @@
         <v>289</v>
       </c>
       <c r="O31" s="1">
-        <v>1116</v>
+        <v>372</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>322</v>
@@ -3294,7 +3286,15 @@
       <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="B32" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>314</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>314</v>
       </c>
@@ -3302,10 +3302,10 @@
         <v>314</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K32" s="1">
         <v>2018</v>
@@ -3320,7 +3320,7 @@
         <v>289</v>
       </c>
       <c r="O32" s="1">
-        <v>7468</v>
+        <v>1116</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>322</v>
@@ -3330,29 +3330,18 @@
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>314</v>
-      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="1" t="s">
         <v>314</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K33" s="1">
         <v>2018</v>
@@ -3367,7 +3356,7 @@
         <v>289</v>
       </c>
       <c r="O33" s="1">
-        <v>6352</v>
+        <v>7468</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>322</v>
@@ -3377,6 +3366,12 @@
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B34" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="D34" s="3" t="s">
         <v>314</v>
       </c>
@@ -3390,10 +3385,10 @@
         <v>314</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K34" s="1">
         <v>2018</v>
@@ -3405,24 +3400,18 @@
         <v>25</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O34" s="1">
-        <v>8.9</v>
+        <v>6352</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>314</v>
+        <v>22</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>314</v>
@@ -3437,10 +3426,10 @@
         <v>314</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K35" s="1">
         <v>2018</v>
@@ -3455,15 +3444,24 @@
         <v>290</v>
       </c>
       <c r="O35" s="1">
-        <v>3.78</v>
+        <v>8.9</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>22</v>
+        <v>98</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>314</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>314</v>
@@ -3475,28 +3473,28 @@
         <v>314</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K36" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O36" s="1">
-        <v>15.7</v>
+        <v>3.78</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.5">
@@ -3513,28 +3511,28 @@
         <v>314</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K37" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O37" s="1">
-        <v>4.26</v>
+        <v>15.7</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.5">
@@ -3551,10 +3549,10 @@
         <v>314</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K38" s="1">
         <v>2018</v>
@@ -3569,42 +3567,48 @@
         <v>290</v>
       </c>
       <c r="O38" s="1">
-        <v>18.39</v>
+        <v>4.26</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E39" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G39" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H39" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K39" s="1">
         <v>2018</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O39" s="1">
-        <v>0</v>
+        <v>18.39</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.5">
@@ -3615,10 +3619,10 @@
         <v>314</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K40" s="1">
         <v>2018</v>
@@ -3647,10 +3651,10 @@
         <v>314</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K41" s="1">
         <v>2018</v>
@@ -3673,46 +3677,34 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>314</v>
+        <v>22</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="K42" s="1">
         <v>2018</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O42" s="1">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.5">
@@ -3735,10 +3727,10 @@
         <v>314</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K43" s="1">
         <v>2018</v>
@@ -3753,16 +3745,25 @@
         <v>290</v>
       </c>
       <c r="O43" s="1">
-        <v>14.2</v>
+        <v>5.6</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="F44" s="1" t="s">
         <v>314</v>
       </c>
@@ -3770,10 +3771,10 @@
         <v>314</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>312</v>
+        <v>113</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K44" s="1">
         <v>2018</v>
@@ -3788,19 +3789,16 @@
         <v>290</v>
       </c>
       <c r="O44" s="1">
-        <v>31504</v>
+        <v>14.2</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="F45" s="1" t="s">
         <v>314</v>
       </c>
@@ -3808,10 +3806,10 @@
         <v>314</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>115</v>
+        <v>312</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>313</v>
+        <v>116</v>
       </c>
       <c r="K45" s="1">
         <v>2018</v>
@@ -3826,42 +3824,48 @@
         <v>290</v>
       </c>
       <c r="O45" s="1">
-        <v>29969</v>
+        <v>31504</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="D46" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="F46" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G46" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H46" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>118</v>
+        <v>313</v>
       </c>
       <c r="K46" s="1">
         <v>2018</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O46" s="1">
-        <v>9.1</v>
+        <v>29969</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.5">
@@ -3872,10 +3876,10 @@
         <v>314</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K47" s="1">
         <v>2018</v>
@@ -3887,13 +3891,13 @@
         <v>119</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O47" s="1">
-        <v>128</v>
+        <v>9.1</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.5">
@@ -3903,32 +3907,29 @@
       <c r="F48" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H48" s="1" t="s">
-        <v>291</v>
+        <v>120</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K48" s="1">
         <v>2018</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O48" s="1">
-        <v>0.38</v>
+        <v>128</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.5">
@@ -3938,11 +3939,14 @@
       <c r="F49" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G49" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H49" s="1" t="s">
-        <v>99</v>
+        <v>291</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="K49" s="1">
         <v>2018</v>
@@ -3957,10 +3961,10 @@
         <v>290</v>
       </c>
       <c r="O49" s="1">
-        <v>8.0299999999999994</v>
+        <v>0.38</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.5">
@@ -3970,14 +3974,11 @@
       <c r="F50" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K50" s="1">
         <v>2018</v>
@@ -3992,7 +3993,7 @@
         <v>290</v>
       </c>
       <c r="O50" s="1">
-        <v>16.18</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>338</v>
@@ -4005,11 +4006,14 @@
       <c r="F51" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G51" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H51" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K51" s="1">
         <v>2018</v>
@@ -4024,7 +4028,7 @@
         <v>290</v>
       </c>
       <c r="O51" s="1">
-        <v>14.7</v>
+        <v>16.18</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>338</v>
@@ -4038,10 +4042,10 @@
         <v>314</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K52" s="1">
         <v>2018</v>
@@ -4056,7 +4060,7 @@
         <v>290</v>
       </c>
       <c r="O52" s="1">
-        <v>15.39</v>
+        <v>14.7</v>
       </c>
       <c r="P52" s="1" t="s">
         <v>338</v>
@@ -4070,10 +4074,10 @@
         <v>314</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K53" s="1">
         <v>2018</v>
@@ -4085,13 +4089,13 @@
         <v>29</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O53" s="1">
-        <v>2092</v>
+        <v>15.39</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.5">
@@ -4101,14 +4105,11 @@
       <c r="F54" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="H54" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K54" s="1">
         <v>2018</v>
@@ -4120,66 +4121,54 @@
         <v>29</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O54" s="1">
-        <v>37.65</v>
+        <v>2092</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>314</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>314</v>
+        <v>268</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="K55" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>126</v>
+        <v>24</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O55" s="1">
-        <v>6.64</v>
+        <v>37.65</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="F56" s="1" t="s">
         <v>314</v>
       </c>
@@ -4187,42 +4176,57 @@
         <v>314</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K56" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>25</v>
+        <v>127</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O56" s="1">
-        <v>11.72</v>
+        <v>6.64</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="B57" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="F57" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G57" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H57" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K57" s="1">
         <v>2018</v>
@@ -4237,7 +4241,7 @@
         <v>290</v>
       </c>
       <c r="O57" s="1">
-        <v>0.68</v>
+        <v>11.72</v>
       </c>
       <c r="P57" s="1" t="s">
         <v>340</v>
@@ -4251,10 +4255,10 @@
         <v>314</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K58" s="1">
         <v>2018</v>
@@ -4269,10 +4273,10 @@
         <v>290</v>
       </c>
       <c r="O58" s="1">
-        <v>8.66</v>
+        <v>0.68</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.5">
@@ -4283,10 +4287,10 @@
         <v>314</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K59" s="1">
         <v>2018</v>
@@ -4301,7 +4305,7 @@
         <v>290</v>
       </c>
       <c r="O59" s="1">
-        <v>19.899999999999999</v>
+        <v>8.66</v>
       </c>
       <c r="P59" s="1" t="s">
         <v>341</v>
@@ -4315,10 +4319,10 @@
         <v>314</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K60" s="1">
         <v>2018</v>
@@ -4333,10 +4337,10 @@
         <v>290</v>
       </c>
       <c r="O60" s="1">
-        <v>673.09</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.5">
@@ -4347,28 +4351,28 @@
         <v>314</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K61" s="1">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>254</v>
+        <v>290</v>
       </c>
       <c r="O61" s="1">
-        <v>1</v>
+        <v>673.09</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.5">
@@ -4379,10 +4383,10 @@
         <v>314</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="K62" s="1">
         <v>2010</v>
@@ -4397,7 +4401,7 @@
         <v>254</v>
       </c>
       <c r="O62" s="1">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="P62" s="1" t="s">
         <v>342</v>
@@ -4410,14 +4414,11 @@
       <c r="F63" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H63" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K63" s="1">
         <v>2010</v>
@@ -4429,10 +4430,10 @@
         <v>141</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="O63" s="1" t="s">
-        <v>308</v>
+        <v>254</v>
+      </c>
+      <c r="O63" s="1">
+        <v>1.1000000000000001</v>
       </c>
       <c r="P63" s="1" t="s">
         <v>342</v>
@@ -4440,48 +4441,51 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G64" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H64" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K64" s="1">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="O64" s="1">
-        <v>6.73</v>
+        <v>292</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
-        <v>123</v>
+        <v>10</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>314</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K65" s="1">
         <v>2018</v>
@@ -4493,13 +4497,13 @@
         <v>149</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O65" s="1">
-        <v>1</v>
+        <v>6.73</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.5">
@@ -4510,10 +4514,10 @@
         <v>314</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K66" s="1">
         <v>2018</v>
@@ -4525,10 +4529,10 @@
         <v>149</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O66" s="1">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="P66" s="1" t="s">
         <v>343</v>
@@ -4542,10 +4546,10 @@
         <v>314</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K67" s="1">
         <v>2018</v>
@@ -4560,7 +4564,7 @@
         <v>290</v>
       </c>
       <c r="O67" s="1">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="P67" s="1" t="s">
         <v>343</v>
@@ -4573,32 +4577,29 @@
       <c r="F68" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G68" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H68" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>307</v>
+        <v>155</v>
       </c>
       <c r="K68" s="1">
         <v>2018</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O68" s="1">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.5">
@@ -4608,29 +4609,32 @@
       <c r="F69" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G69" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H69" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>160</v>
+        <v>307</v>
       </c>
       <c r="K69" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O69" s="1">
-        <v>0.81</v>
+        <v>0.15</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.5">
@@ -4641,10 +4645,10 @@
         <v>314</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K70" s="1">
         <v>2019</v>
@@ -4673,10 +4677,10 @@
         <v>314</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K71" s="1">
         <v>2019</v>
@@ -4691,10 +4695,10 @@
         <v>290</v>
       </c>
       <c r="O71" s="1">
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.5">
@@ -4705,10 +4709,10 @@
         <v>314</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K72" s="1">
         <v>2019</v>
@@ -4720,13 +4724,13 @@
         <v>162</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O72" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>322</v>
+        <v>346</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.5">
@@ -4737,10 +4741,10 @@
         <v>314</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K73" s="1">
         <v>2019</v>
@@ -4752,13 +4756,13 @@
         <v>162</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O73" s="1">
-        <v>13.22</v>
+        <v>21</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.5">
@@ -4769,10 +4773,10 @@
         <v>314</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K74" s="1">
         <v>2019</v>
@@ -4787,10 +4791,10 @@
         <v>290</v>
       </c>
       <c r="O74" s="1">
-        <v>27.39</v>
+        <v>13.22</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.5">
@@ -4801,10 +4805,10 @@
         <v>314</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="K75" s="1">
         <v>2019</v>
@@ -4816,13 +4820,13 @@
         <v>162</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O75" s="1">
-        <v>1</v>
+        <v>27.39</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.5">
@@ -4833,10 +4837,10 @@
         <v>314</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K76" s="1">
         <v>2019</v>
@@ -4848,13 +4852,13 @@
         <v>162</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O76" s="1">
-        <v>18.04</v>
+        <v>1</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.5">
@@ -4865,10 +4869,10 @@
         <v>314</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K77" s="1">
         <v>2019</v>
@@ -4883,10 +4887,10 @@
         <v>290</v>
       </c>
       <c r="O77" s="1">
-        <v>35.340000000000003</v>
+        <v>18.04</v>
       </c>
       <c r="P77" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.5">
@@ -4897,10 +4901,10 @@
         <v>314</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K78" s="1">
         <v>2019</v>
@@ -4912,16 +4916,16 @@
         <v>162</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O78" s="1">
-        <v>0</v>
+        <v>35.340000000000003</v>
       </c>
       <c r="P78" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>123</v>
       </c>
@@ -4929,10 +4933,10 @@
         <v>314</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>316</v>
+        <v>179</v>
       </c>
       <c r="K79" s="1">
         <v>2019</v>
@@ -4944,16 +4948,16 @@
         <v>162</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O79" s="1">
         <v>0</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.5">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>123</v>
       </c>
@@ -4961,10 +4965,10 @@
         <v>314</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>182</v>
+        <v>316</v>
       </c>
       <c r="K80" s="1">
         <v>2019</v>
@@ -4976,13 +4980,13 @@
         <v>162</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O80" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.5">
@@ -4993,10 +4997,10 @@
         <v>314</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K81" s="1">
         <v>2019</v>
@@ -5025,10 +5029,10 @@
         <v>314</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>317</v>
+        <v>184</v>
       </c>
       <c r="K82" s="1">
         <v>2019</v>
@@ -5040,13 +5044,13 @@
         <v>162</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O82" s="1">
-        <v>1744.66</v>
+        <v>2</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>350</v>
+        <v>322</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.5">
@@ -5057,10 +5061,10 @@
         <v>314</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>187</v>
+        <v>317</v>
       </c>
       <c r="K83" s="1">
         <v>2019</v>
@@ -5072,13 +5076,13 @@
         <v>162</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O83" s="1">
-        <v>0</v>
+        <v>1744.66</v>
       </c>
       <c r="P83" s="1" t="s">
-        <v>322</v>
+        <v>350</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.5">
@@ -5089,10 +5093,10 @@
         <v>314</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K84" s="1">
         <v>2019</v>
@@ -5121,10 +5125,10 @@
         <v>314</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>318</v>
+        <v>189</v>
       </c>
       <c r="K85" s="1">
         <v>2019</v>
@@ -5136,13 +5140,13 @@
         <v>162</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="O85" s="1" t="s">
-        <v>319</v>
+        <v>289</v>
+      </c>
+      <c r="O85" s="1">
+        <v>0</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.5">
@@ -5153,10 +5157,10 @@
         <v>314</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>192</v>
+        <v>318</v>
       </c>
       <c r="K86" s="1">
         <v>2019</v>
@@ -5168,13 +5172,13 @@
         <v>162</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="O86" s="1">
-        <v>0</v>
+        <v>290</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>322</v>
+        <v>351</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.5">
@@ -5185,10 +5189,10 @@
         <v>314</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K87" s="1">
         <v>2019</v>
@@ -5217,10 +5221,10 @@
         <v>314</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K88" s="1">
         <v>2019</v>
@@ -5232,13 +5236,13 @@
         <v>162</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O88" s="1">
         <v>0</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>352</v>
+        <v>322</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.5">
@@ -5249,10 +5253,10 @@
         <v>314</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K89" s="1">
         <v>2019</v>
@@ -5264,13 +5268,13 @@
         <v>162</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O89" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>322</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.5">
@@ -5281,10 +5285,10 @@
         <v>314</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K90" s="1">
         <v>2019</v>
@@ -5299,7 +5303,7 @@
         <v>289</v>
       </c>
       <c r="O90" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P90" s="1" t="s">
         <v>322</v>
@@ -5313,10 +5317,10 @@
         <v>314</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K91" s="1">
         <v>2019</v>
@@ -5328,13 +5332,13 @@
         <v>162</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O91" s="1">
-        <v>148.18</v>
+        <v>3</v>
       </c>
       <c r="P91" s="1" t="s">
-        <v>353</v>
+        <v>322</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.5">
@@ -5345,10 +5349,10 @@
         <v>314</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K92" s="1">
         <v>2019</v>
@@ -5360,13 +5364,13 @@
         <v>162</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O92" s="1">
-        <v>0</v>
+        <v>148.18</v>
       </c>
       <c r="P92" s="1" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.5">
@@ -5377,10 +5381,10 @@
         <v>314</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K93" s="1">
         <v>2019</v>
@@ -5409,10 +5413,10 @@
         <v>314</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K94" s="1">
         <v>2019</v>
@@ -5424,13 +5428,13 @@
         <v>162</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O94" s="1">
-        <v>165.18</v>
+        <v>0</v>
       </c>
       <c r="P94" s="1" t="s">
-        <v>354</v>
+        <v>322</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.5">
@@ -5441,10 +5445,10 @@
         <v>314</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K95" s="1">
         <v>2019</v>
@@ -5456,13 +5460,13 @@
         <v>162</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O95" s="1">
-        <v>0</v>
+        <v>165.18</v>
       </c>
       <c r="P95" s="1" t="s">
-        <v>322</v>
+        <v>354</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.5">
@@ -5473,10 +5477,10 @@
         <v>314</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K96" s="1">
         <v>2019</v>
@@ -5505,25 +5509,25 @@
         <v>314</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K97" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>215</v>
+        <v>161</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>216</v>
+        <v>162</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O97" s="1">
-        <v>10.23</v>
+        <v>0</v>
       </c>
       <c r="P97" s="1" t="s">
         <v>322</v>
@@ -5537,10 +5541,10 @@
         <v>314</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K98" s="1">
         <v>2020</v>
@@ -5555,10 +5559,10 @@
         <v>290</v>
       </c>
       <c r="O98" s="1">
-        <v>19.16</v>
+        <v>10.23</v>
       </c>
       <c r="P98" s="1" t="s">
-        <v>355</v>
+        <v>322</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.5">
@@ -5569,10 +5573,10 @@
         <v>314</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>302</v>
+        <v>217</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K99" s="1">
         <v>2020</v>
@@ -5584,13 +5588,13 @@
         <v>216</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O99" s="1">
-        <v>17</v>
+        <v>19.16</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>322</v>
+        <v>355</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.5">
@@ -5601,25 +5605,25 @@
         <v>314</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K100" s="1">
         <v>2020</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O100" s="1">
-        <v>0.31</v>
+        <v>17</v>
       </c>
       <c r="P100" s="1" t="s">
         <v>322</v>
@@ -5633,10 +5637,10 @@
         <v>314</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K101" s="1">
         <v>2020</v>
@@ -5651,10 +5655,10 @@
         <v>290</v>
       </c>
       <c r="O101" s="1">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>356</v>
+        <v>322</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.5">
@@ -5665,10 +5669,10 @@
         <v>314</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K102" s="1">
         <v>2020</v>
@@ -5680,13 +5684,13 @@
         <v>221</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O102" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.5">
@@ -5697,25 +5701,25 @@
         <v>314</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K103" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O103" s="1">
-        <v>0.84</v>
+        <v>6</v>
       </c>
       <c r="P103" s="1" t="s">
         <v>322</v>
@@ -5729,10 +5733,10 @@
         <v>314</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>226</v>
+        <v>293</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="K104" s="1">
         <v>2019</v>
@@ -5747,10 +5751,10 @@
         <v>290</v>
       </c>
       <c r="O104" s="1">
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.5">
@@ -5761,10 +5765,10 @@
         <v>314</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>294</v>
+        <v>226</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K105" s="1">
         <v>2019</v>
@@ -5776,13 +5780,13 @@
         <v>225</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O105" s="1">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>322</v>
+        <v>357</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.5">
@@ -5793,25 +5797,25 @@
         <v>314</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K106" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O106" s="1">
-        <v>0.2</v>
+        <v>58</v>
       </c>
       <c r="P106" s="1" t="s">
         <v>322</v>
@@ -5825,10 +5829,10 @@
         <v>314</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>232</v>
+        <v>295</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="K107" s="1">
         <v>2020</v>
@@ -5843,10 +5847,10 @@
         <v>290</v>
       </c>
       <c r="O107" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>358</v>
+        <v>322</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.5">
@@ -5857,10 +5861,10 @@
         <v>314</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>296</v>
+        <v>232</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K108" s="1">
         <v>2020</v>
@@ -5872,13 +5876,13 @@
         <v>231</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O108" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>322</v>
+        <v>358</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.5">
@@ -5889,10 +5893,10 @@
         <v>314</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K109" s="1">
         <v>2020</v>
@@ -5904,13 +5908,13 @@
         <v>231</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O109" s="1">
-        <v>4.99</v>
+        <v>3</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.5">
@@ -5921,10 +5925,10 @@
         <v>314</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K110" s="1">
         <v>2020</v>
@@ -5939,10 +5943,10 @@
         <v>290</v>
       </c>
       <c r="O110" s="1">
-        <v>17.760000000000002</v>
+        <v>4.99</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>359</v>
+        <v>323</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.5">
@@ -5953,10 +5957,10 @@
         <v>314</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K111" s="1">
         <v>2020</v>
@@ -5968,13 +5972,13 @@
         <v>231</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O111" s="1">
-        <v>4</v>
+        <v>17.760000000000002</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>322</v>
+        <v>359</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.5">
@@ -5985,25 +5989,25 @@
         <v>314</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K112" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="M112" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O112" s="1">
-        <v>13.12</v>
+        <v>4</v>
       </c>
       <c r="P112" s="1" t="s">
         <v>322</v>
@@ -6017,10 +6021,10 @@
         <v>314</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K113" s="1">
         <v>2021</v>
@@ -6035,10 +6039,10 @@
         <v>290</v>
       </c>
       <c r="O113" s="1">
-        <v>27.39</v>
+        <v>13.12</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.5">
@@ -6049,10 +6053,10 @@
         <v>314</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K114" s="1">
         <v>2021</v>
@@ -6064,13 +6068,13 @@
         <v>240</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O114" s="1">
-        <v>1</v>
+        <v>27.39</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>322</v>
+        <v>360</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.5">
@@ -6081,28 +6085,28 @@
         <v>314</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>243</v>
+        <v>301</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="K115" s="1">
-        <v>2010</v>
+        <v>2021</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="N115" s="1" t="s">
         <v>289</v>
       </c>
       <c r="O115" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.5">
@@ -6113,10 +6117,10 @@
         <v>314</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="K116" s="1">
         <v>2010</v>
@@ -6131,7 +6135,7 @@
         <v>289</v>
       </c>
       <c r="O116" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="P116" s="1" t="s">
         <v>342</v>
@@ -6144,14 +6148,11 @@
       <c r="F117" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G117" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H117" s="1" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K117" s="1">
         <v>2010</v>
@@ -6163,13 +6164,13 @@
         <v>246</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O117" s="1">
-        <v>133.41999999999999</v>
+        <v>4</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.5">
@@ -6179,11 +6180,14 @@
       <c r="F118" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G118" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H118" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K118" s="1">
         <v>2010</v>
@@ -6198,45 +6202,42 @@
         <v>290</v>
       </c>
       <c r="O118" s="1">
-        <v>41.05</v>
+        <v>133.41999999999999</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
-        <v>251</v>
+        <v>123</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G119" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="H119" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="K119" s="1">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>285</v>
+        <v>246</v>
       </c>
       <c r="N119" s="1" t="s">
         <v>290</v>
       </c>
       <c r="O119" s="1">
-        <v>1.17</v>
+        <v>41.05</v>
       </c>
       <c r="P119" s="1" t="s">
-        <v>344</v>
+        <v>362</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.5">
@@ -6250,10 +6251,10 @@
         <v>314</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K120" s="1">
         <v>2014</v>
@@ -6268,7 +6269,7 @@
         <v>290</v>
       </c>
       <c r="O120" s="1">
-        <v>0.54</v>
+        <v>1.17</v>
       </c>
       <c r="P120" s="1" t="s">
         <v>344</v>
@@ -6285,10 +6286,10 @@
         <v>314</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K121" s="1">
         <v>2014</v>
@@ -6303,7 +6304,7 @@
         <v>290</v>
       </c>
       <c r="O121" s="1">
-        <v>-0.06</v>
+        <v>0.54</v>
       </c>
       <c r="P121" s="1" t="s">
         <v>344</v>
@@ -6320,10 +6321,10 @@
         <v>314</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K122" s="1">
         <v>2014</v>
@@ -6338,7 +6339,7 @@
         <v>290</v>
       </c>
       <c r="O122" s="1">
-        <v>0.59</v>
+        <v>-0.06</v>
       </c>
       <c r="P122" s="1" t="s">
         <v>344</v>
@@ -6351,29 +6352,32 @@
       <c r="F123" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="G123" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="H123" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="K123" s="1">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>253</v>
+        <v>286</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>253</v>
+        <v>285</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>254</v>
+        <v>290</v>
       </c>
       <c r="O123" s="1">
-        <v>3</v>
+        <v>0.59</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.5">
@@ -6384,28 +6388,28 @@
         <v>314</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K124" s="1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M124" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>26</v>
+        <v>254</v>
       </c>
       <c r="O124" s="1">
-        <v>0.43</v>
+        <v>3</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.5">
@@ -6416,10 +6420,10 @@
         <v>314</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="K125" s="1">
         <v>2018</v>
@@ -6434,10 +6438,10 @@
         <v>26</v>
       </c>
       <c r="O125" s="1">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.5">
@@ -6448,10 +6452,10 @@
         <v>314</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K126" s="1">
         <v>2018</v>
@@ -6466,10 +6470,10 @@
         <v>26</v>
       </c>
       <c r="O126" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="P126" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.5">
@@ -6480,10 +6484,10 @@
         <v>314</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K127" s="1">
         <v>2018</v>
@@ -6498,10 +6502,10 @@
         <v>26</v>
       </c>
       <c r="O127" s="1">
-        <v>0.61</v>
+        <v>0.2</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.5">
@@ -6512,10 +6516,10 @@
         <v>314</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K128" s="1">
         <v>2018</v>
@@ -6530,9 +6534,41 @@
         <v>26</v>
       </c>
       <c r="O128" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="P128" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A129" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K129" s="1">
+        <v>2018</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O129" s="1">
         <v>0.38</v>
       </c>
-      <c r="P128" s="1" t="s">
+      <c r="P129" s="1" t="s">
         <v>365</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added state level table, updated dictionaries
</commit_message>
<xml_diff>
--- a/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
+++ b/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\data_final\consolidated\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E495AB0-6C07-4EE0-8E4C-FE5B34A23C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586AF102-25CC-41D2-BA40-5486530C345E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="11686" windowHeight="14483" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22943" yWindow="-14655" windowWidth="38595" windowHeight="21795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tractsDataDictionary" sheetId="1" r:id="rId1"/>
@@ -1626,13 +1626,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1991,7 +1992,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2004,56 +2005,56 @@
     <col min="11" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="4">
         <v>1980</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="4">
         <v>1990</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="4">
         <v>2000</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="4">
         <v>2010</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated analysis column; this likely needs a double check
</commit_message>
<xml_diff>
--- a/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
+++ b/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\data_final\consolidated\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36721559-7E78-4028-9E00-AEAFB97BCD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6081D5F8-269A-4E07-99DA-FC220BB0D6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22943" yWindow="-14655" windowWidth="38595" windowHeight="21795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="390">
   <si>
     <t>Theme</t>
   </si>
@@ -836,9 +836,6 @@
     <t>Analysis</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>ZIP</t>
   </si>
   <si>
@@ -884,9 +881,6 @@
     <t>Raw Urban Core Opportunity Index (https://sdohatlas.github.io/)</t>
   </si>
   <si>
-    <t>Raw MICA Index (https://sdohatlas.github.io/)</t>
-  </si>
-  <si>
     <t>GeoDa Data and Lab; Spatial Deterimants of Health Atlas</t>
   </si>
   <si>
@@ -1206,6 +1200,9 @@
   </si>
   <si>
     <t>Health03</t>
+  </si>
+  <si>
+    <t>Raw Mixed Immigrant Cohesion and Accessibility (MICA) Index (https://sdohatlas.github.io/)</t>
   </si>
 </sst>
 </file>
@@ -2060,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2089,7 +2086,7 @@
         <v>2010</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>266</v>
@@ -2110,7 +2107,7 @@
         <v>5</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>6</v>
@@ -2119,7 +2116,7 @@
         <v>7</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>8</v>
@@ -2148,10 +2145,10 @@
         <v>14</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.5">
@@ -2177,10 +2174,10 @@
         <v>14</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.5">
@@ -2188,19 +2185,19 @@
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J4" s="1">
         <v>2018</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>14</v>
@@ -2209,7 +2206,7 @@
         <v>36526</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.5">
@@ -2235,10 +2232,10 @@
         <v>14</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.5">
@@ -2264,10 +2261,10 @@
         <v>14</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.5">
@@ -2275,28 +2272,28 @@
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J7" s="1">
         <v>2018</v>
@@ -2308,16 +2305,16 @@
         <v>24</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O7" s="1">
         <v>9744</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.5">
@@ -2326,13 +2323,13 @@
       </c>
       <c r="D8" s="3"/>
       <c r="F8" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J8" s="1">
         <v>2018</v>
@@ -2344,10 +2341,10 @@
         <v>24</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O8" s="1">
         <v>52</v>
@@ -2359,10 +2356,10 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>26</v>
@@ -2380,16 +2377,16 @@
         <v>28</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O9" s="1">
         <v>9670</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.5">
@@ -2397,19 +2394,19 @@
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>29</v>
@@ -2427,16 +2424,16 @@
         <v>24</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O10" s="1">
         <v>4532</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.5">
@@ -2445,7 +2442,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="F11" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>30</v>
@@ -2463,16 +2460,16 @@
         <v>28</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O11" s="1">
         <v>5556</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.5">
@@ -2480,22 +2477,22 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -2513,16 +2510,16 @@
         <v>24</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O12" s="1">
         <v>80.290000000000006</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.5">
@@ -2530,22 +2527,22 @@
         <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>34</v>
@@ -2563,16 +2560,16 @@
         <v>24</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O13" s="1">
         <v>13.78</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.5">
@@ -2580,22 +2577,22 @@
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>36</v>
@@ -2613,16 +2610,16 @@
         <v>24</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O14" s="1">
         <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.5">
@@ -2630,22 +2627,22 @@
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>38</v>
@@ -2663,16 +2660,16 @@
         <v>24</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O15" s="1">
         <v>0.38</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.5">
@@ -2680,22 +2677,22 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>40</v>
@@ -2713,16 +2710,16 @@
         <v>24</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O16" s="1">
         <v>0</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.5">
@@ -2730,22 +2727,22 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>42</v>
@@ -2763,16 +2760,16 @@
         <v>24</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O17" s="1">
         <v>5.55</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.5">
@@ -2780,22 +2777,22 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>44</v>
@@ -2813,16 +2810,16 @@
         <v>24</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O18" s="1">
         <v>8.18</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.5">
@@ -2831,16 +2828,16 @@
       </c>
       <c r="D19" s="3"/>
       <c r="F19" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J19" s="1">
         <v>2018</v>
@@ -2852,13 +2849,13 @@
         <v>24</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O19" s="1">
         <v>0.23</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.5">
@@ -2866,22 +2863,22 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>47</v>
@@ -2899,16 +2896,16 @@
         <v>24</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O20" s="1">
         <v>14.63</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.5">
@@ -2916,19 +2913,19 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>49</v>
@@ -2946,16 +2943,16 @@
         <v>24</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O21" s="1">
         <v>66.83</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.5">
@@ -2963,19 +2960,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>51</v>
@@ -2993,16 +2990,16 @@
         <v>24</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O22" s="1">
         <v>11.45</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.5">
@@ -3010,19 +3007,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>53</v>
@@ -3040,16 +3037,16 @@
         <v>24</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O23" s="1">
         <v>607</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.5">
@@ -3057,19 +3054,19 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>55</v>
@@ -3087,16 +3084,16 @@
         <v>24</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O24" s="1">
         <v>1070</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.5">
@@ -3104,19 +3101,19 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>57</v>
@@ -3134,16 +3131,16 @@
         <v>24</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O25" s="1">
         <v>722</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.5">
@@ -3151,19 +3148,19 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>59</v>
@@ -3181,16 +3178,16 @@
         <v>24</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O26" s="1">
         <v>704</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.5">
@@ -3198,19 +3195,19 @@
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>61</v>
@@ -3228,16 +3225,16 @@
         <v>24</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O27" s="1">
         <v>4835</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.5">
@@ -3245,16 +3242,16 @@
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>63</v>
@@ -3272,16 +3269,16 @@
         <v>24</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O28" s="1">
         <v>495</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.5">
@@ -3289,16 +3286,16 @@
         <v>21</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>65</v>
@@ -3316,16 +3313,16 @@
         <v>24</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O29" s="1">
         <v>531</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.5">
@@ -3333,19 +3330,19 @@
         <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>67</v>
@@ -3363,16 +3360,16 @@
         <v>24</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O30" s="1">
         <v>718</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.5">
@@ -3380,19 +3377,19 @@
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>69</v>
@@ -3410,16 +3407,16 @@
         <v>24</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O31" s="1">
         <v>372</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.5">
@@ -3427,19 +3424,19 @@
         <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>71</v>
@@ -3457,16 +3454,16 @@
         <v>24</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O32" s="1">
         <v>1116</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.5">
@@ -3475,10 +3472,10 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>73</v>
@@ -3496,16 +3493,16 @@
         <v>24</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O33" s="1">
         <v>7468</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.5">
@@ -3513,22 +3510,22 @@
         <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>75</v>
@@ -3546,16 +3543,16 @@
         <v>24</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O34" s="1">
         <v>6352</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.5">
@@ -3563,16 +3560,16 @@
         <v>21</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>77</v>
@@ -3590,16 +3587,16 @@
         <v>24</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O35" s="1">
         <v>8.9</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.5">
@@ -3607,22 +3604,22 @@
         <v>97</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>79</v>
@@ -3640,16 +3637,16 @@
         <v>24</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O36" s="1">
         <v>3.78</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.5">
@@ -3657,13 +3654,13 @@
         <v>21</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>81</v>
@@ -3681,16 +3678,16 @@
         <v>84</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O37" s="1">
         <v>15.7</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.5">
@@ -3698,13 +3695,13 @@
         <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>85</v>
@@ -3722,16 +3719,16 @@
         <v>28</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O38" s="1">
         <v>4.26</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.5">
@@ -3739,13 +3736,13 @@
         <v>21</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>87</v>
@@ -3763,16 +3760,16 @@
         <v>28</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O39" s="1">
         <v>18.39</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.5">
@@ -3780,7 +3777,7 @@
         <v>21</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>89</v>
@@ -3798,16 +3795,16 @@
         <v>92</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O40" s="1">
         <v>0</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.5">
@@ -3815,7 +3812,7 @@
         <v>21</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>93</v>
@@ -3833,16 +3830,16 @@
         <v>92</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O41" s="1">
         <v>0</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.5">
@@ -3850,7 +3847,7 @@
         <v>21</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>95</v>
@@ -3868,16 +3865,16 @@
         <v>92</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O42" s="1">
         <v>0</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.5">
@@ -3885,19 +3882,19 @@
         <v>97</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>110</v>
@@ -3915,16 +3912,16 @@
         <v>28</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O43" s="1">
         <v>5.6</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.5">
@@ -3932,19 +3929,19 @@
         <v>97</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>112</v>
@@ -3962,16 +3959,16 @@
         <v>28</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O44" s="1">
         <v>14.2</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.5">
@@ -3979,13 +3976,13 @@
         <v>97</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>115</v>
@@ -4000,13 +3997,13 @@
         <v>28</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O45" s="1">
         <v>31504</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.5">
@@ -4014,19 +4011,19 @@
         <v>97</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J46" s="1">
         <v>2018</v>
@@ -4038,16 +4035,16 @@
         <v>28</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O46" s="1">
         <v>29969</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.5">
@@ -4055,7 +4052,7 @@
         <v>97</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>116</v>
@@ -4073,16 +4070,16 @@
         <v>118</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O47" s="1">
         <v>9.1</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.5">
@@ -4090,7 +4087,7 @@
         <v>97</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>119</v>
@@ -4108,16 +4105,16 @@
         <v>118</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O48" s="1">
         <v>128</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.5">
@@ -4125,13 +4122,13 @@
         <v>97</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>121</v>
@@ -4146,13 +4143,13 @@
         <v>28</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O49" s="1">
         <v>0.38</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.5">
@@ -4160,7 +4157,7 @@
         <v>97</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>98</v>
@@ -4178,16 +4175,16 @@
         <v>28</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O50" s="1">
         <v>8.0299999999999994</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.5">
@@ -4195,10 +4192,10 @@
         <v>97</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>100</v>
@@ -4216,16 +4213,16 @@
         <v>28</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O51" s="1">
         <v>16.18</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.5">
@@ -4233,7 +4230,7 @@
         <v>97</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>102</v>
@@ -4251,16 +4248,16 @@
         <v>28</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O52" s="1">
         <v>14.7</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.5">
@@ -4268,7 +4265,7 @@
         <v>97</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>104</v>
@@ -4286,16 +4283,16 @@
         <v>28</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O53" s="1">
         <v>15.39</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.5">
@@ -4303,7 +4300,7 @@
         <v>97</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>106</v>
@@ -4321,16 +4318,16 @@
         <v>28</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O54" s="1">
         <v>2092</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.5">
@@ -4338,10 +4335,10 @@
         <v>97</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>267</v>
+        <v>311</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>108</v>
@@ -4359,16 +4356,16 @@
         <v>28</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O55" s="1">
         <v>37.65</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.5">
@@ -4376,10 +4373,10 @@
         <v>122</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>123</v>
@@ -4397,16 +4394,16 @@
         <v>126</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O56" s="1">
         <v>6.64</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.5">
@@ -4414,22 +4411,22 @@
         <v>122</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>127</v>
@@ -4447,16 +4444,16 @@
         <v>24</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O57" s="1">
         <v>11.72</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.5">
@@ -4464,7 +4461,7 @@
         <v>122</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>129</v>
@@ -4482,16 +4479,16 @@
         <v>24</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O58" s="1">
         <v>0.68</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.5">
@@ -4499,7 +4496,7 @@
         <v>122</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>131</v>
@@ -4517,16 +4514,16 @@
         <v>24</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O59" s="1">
         <v>8.66</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.5">
@@ -4534,7 +4531,7 @@
         <v>122</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>133</v>
@@ -4552,16 +4549,16 @@
         <v>24</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O60" s="1">
         <v>19.899999999999999</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.5">
@@ -4569,7 +4566,7 @@
         <v>122</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>135</v>
@@ -4587,16 +4584,16 @@
         <v>24</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O61" s="1">
         <v>673.09</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.5">
@@ -4604,7 +4601,7 @@
         <v>122</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>137</v>
@@ -4622,7 +4619,7 @@
         <v>140</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>253</v>
@@ -4631,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.5">
@@ -4639,7 +4636,7 @@
         <v>122</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>141</v>
@@ -4657,7 +4654,7 @@
         <v>140</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="N63" s="1" t="s">
         <v>253</v>
@@ -4666,7 +4663,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.5">
@@ -4674,10 +4671,10 @@
         <v>122</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>143</v>
@@ -4695,16 +4692,16 @@
         <v>140</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.5">
@@ -4712,7 +4709,7 @@
         <v>9</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>145</v>
@@ -4730,16 +4727,16 @@
         <v>148</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O65" s="1">
         <v>6.73</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.5">
@@ -4747,7 +4744,7 @@
         <v>122</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>149</v>
@@ -4765,16 +4762,16 @@
         <v>148</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O66" s="1">
         <v>1</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.5">
@@ -4782,7 +4779,7 @@
         <v>122</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>151</v>
@@ -4800,16 +4797,16 @@
         <v>148</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O67" s="1">
         <v>0.15</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.5">
@@ -4817,7 +4814,7 @@
         <v>122</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>153</v>
@@ -4835,16 +4832,16 @@
         <v>148</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O68" s="1">
         <v>0</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.5">
@@ -4852,16 +4849,16 @@
         <v>122</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>155</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J69" s="1">
         <v>2018</v>
@@ -4873,16 +4870,16 @@
         <v>157</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O69" s="1">
         <v>0.15</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.5">
@@ -4890,7 +4887,7 @@
         <v>122</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>158</v>
@@ -4908,16 +4905,16 @@
         <v>161</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O70" s="1">
         <v>0.81</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.5">
@@ -4925,7 +4922,7 @@
         <v>122</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>162</v>
@@ -4943,16 +4940,16 @@
         <v>161</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O71" s="1">
         <v>0.81</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.5">
@@ -4960,7 +4957,10 @@
         <v>122</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>164</v>
@@ -4978,16 +4978,16 @@
         <v>161</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O72" s="1">
         <v>0</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.5">
@@ -4995,7 +4995,7 @@
         <v>122</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>166</v>
@@ -5013,16 +5013,16 @@
         <v>161</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O73" s="1">
         <v>21</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.5">
@@ -5030,7 +5030,7 @@
         <v>122</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>168</v>
@@ -5048,16 +5048,16 @@
         <v>161</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O74" s="1">
         <v>13.22</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.5">
@@ -5065,7 +5065,10 @@
         <v>122</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>170</v>
@@ -5083,16 +5086,16 @@
         <v>161</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O75" s="1">
         <v>27.39</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.5">
@@ -5100,7 +5103,7 @@
         <v>122</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>172</v>
@@ -5118,16 +5121,16 @@
         <v>161</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O76" s="1">
         <v>1</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.5">
@@ -5135,7 +5138,7 @@
         <v>122</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>173</v>
@@ -5153,16 +5156,16 @@
         <v>161</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O77" s="1">
         <v>18.04</v>
       </c>
       <c r="P77" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.5">
@@ -5170,7 +5173,10 @@
         <v>122</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>175</v>
@@ -5188,16 +5194,16 @@
         <v>161</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O78" s="1">
         <v>35.340000000000003</v>
       </c>
       <c r="P78" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.5">
@@ -5205,7 +5211,7 @@
         <v>122</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>177</v>
@@ -5223,16 +5229,16 @@
         <v>161</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O79" s="1">
         <v>0</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="80" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
@@ -5240,13 +5246,16 @@
         <v>122</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>179</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J80" s="1">
         <v>2019</v>
@@ -5258,16 +5267,16 @@
         <v>161</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O80" s="1">
         <v>0</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.5">
@@ -5275,7 +5284,7 @@
         <v>122</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>180</v>
@@ -5293,16 +5302,16 @@
         <v>161</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O81" s="1">
         <v>2</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.5">
@@ -5310,7 +5319,7 @@
         <v>122</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>182</v>
@@ -5328,16 +5337,16 @@
         <v>161</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O82" s="1">
         <v>2</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.5">
@@ -5345,13 +5354,16 @@
         <v>122</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>184</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J83" s="1">
         <v>2019</v>
@@ -5363,16 +5375,16 @@
         <v>161</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O83" s="1">
         <v>1744.66</v>
       </c>
       <c r="P83" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.5">
@@ -5380,7 +5392,7 @@
         <v>122</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>185</v>
@@ -5398,16 +5410,16 @@
         <v>161</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O84" s="1">
         <v>0</v>
       </c>
       <c r="P84" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.5">
@@ -5415,7 +5427,7 @@
         <v>122</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>187</v>
@@ -5433,16 +5445,16 @@
         <v>161</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O85" s="1">
         <v>0</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.5">
@@ -5450,13 +5462,16 @@
         <v>122</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>189</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J86" s="1">
         <v>2019</v>
@@ -5468,16 +5483,16 @@
         <v>161</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.5">
@@ -5485,7 +5500,7 @@
         <v>122</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>190</v>
@@ -5503,16 +5518,16 @@
         <v>161</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O87" s="1">
         <v>0</v>
       </c>
       <c r="P87" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.5">
@@ -5520,7 +5535,7 @@
         <v>122</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>192</v>
@@ -5538,16 +5553,16 @@
         <v>161</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O88" s="1">
         <v>0</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.5">
@@ -5555,7 +5570,10 @@
         <v>122</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>194</v>
@@ -5573,16 +5591,16 @@
         <v>161</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O89" s="1">
         <v>0</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.5">
@@ -5590,7 +5608,7 @@
         <v>122</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>196</v>
@@ -5608,16 +5626,16 @@
         <v>161</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O90" s="1">
         <v>4</v>
       </c>
       <c r="P90" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.5">
@@ -5625,7 +5643,7 @@
         <v>122</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>198</v>
@@ -5643,16 +5661,16 @@
         <v>161</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O91" s="1">
         <v>3</v>
       </c>
       <c r="P91" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.5">
@@ -5660,7 +5678,10 @@
         <v>122</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>200</v>
@@ -5678,16 +5699,16 @@
         <v>161</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O92" s="1">
         <v>148.18</v>
       </c>
       <c r="P92" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.5">
@@ -5695,7 +5716,7 @@
         <v>122</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>202</v>
@@ -5713,16 +5734,16 @@
         <v>161</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O93" s="1">
         <v>0</v>
       </c>
       <c r="P93" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.5">
@@ -5730,7 +5751,7 @@
         <v>122</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>204</v>
@@ -5748,16 +5769,16 @@
         <v>161</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O94" s="1">
         <v>0</v>
       </c>
       <c r="P94" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.5">
@@ -5765,7 +5786,10 @@
         <v>122</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>206</v>
@@ -5783,16 +5807,16 @@
         <v>161</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O95" s="1">
         <v>165.18</v>
       </c>
       <c r="P95" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.5">
@@ -5800,7 +5824,7 @@
         <v>122</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>208</v>
@@ -5818,16 +5842,16 @@
         <v>161</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O96" s="1">
         <v>0</v>
       </c>
       <c r="P96" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.5">
@@ -5835,7 +5859,7 @@
         <v>122</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>210</v>
@@ -5853,16 +5877,16 @@
         <v>161</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O97" s="1">
         <v>0</v>
       </c>
       <c r="P97" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.5">
@@ -5870,7 +5894,7 @@
         <v>122</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>212</v>
@@ -5888,16 +5912,16 @@
         <v>215</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O98" s="1">
         <v>10.23</v>
       </c>
       <c r="P98" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.5">
@@ -5905,7 +5929,10 @@
         <v>122</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>216</v>
@@ -5923,16 +5950,16 @@
         <v>215</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O99" s="1">
         <v>19.16</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.5">
@@ -5940,10 +5967,10 @@
         <v>122</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>218</v>
@@ -5958,16 +5985,16 @@
         <v>215</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O100" s="1">
         <v>17</v>
       </c>
       <c r="P100" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.5">
@@ -5975,10 +6002,10 @@
         <v>122</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>219</v>
@@ -5993,16 +6020,16 @@
         <v>220</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O101" s="1">
         <v>0.31</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.5">
@@ -6010,10 +6037,13 @@
         <v>122</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>221</v>
@@ -6028,16 +6058,16 @@
         <v>220</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O102" s="1">
         <v>0</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.5">
@@ -6045,10 +6075,10 @@
         <v>122</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>222</v>
@@ -6063,16 +6093,16 @@
         <v>220</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O103" s="1">
         <v>6</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.5">
@@ -6080,10 +6110,10 @@
         <v>122</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>223</v>
@@ -6098,16 +6128,16 @@
         <v>224</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O104" s="1">
         <v>0.84</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.5">
@@ -6115,7 +6145,10 @@
         <v>122</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>225</v>
@@ -6133,16 +6166,16 @@
         <v>224</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O105" s="1">
         <v>0</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.5">
@@ -6150,10 +6183,10 @@
         <v>122</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>227</v>
@@ -6168,16 +6201,16 @@
         <v>224</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O106" s="1">
         <v>58</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.5">
@@ -6185,10 +6218,10 @@
         <v>122</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>228</v>
@@ -6203,16 +6236,16 @@
         <v>230</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O107" s="1">
         <v>0.2</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.5">
@@ -6220,7 +6253,10 @@
         <v>122</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>231</v>
@@ -6238,16 +6274,16 @@
         <v>230</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O108" s="1">
         <v>0</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.5">
@@ -6255,10 +6291,10 @@
         <v>122</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>233</v>
@@ -6273,16 +6309,16 @@
         <v>230</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O109" s="1">
         <v>3</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.5">
@@ -6290,10 +6326,10 @@
         <v>122</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>234</v>
@@ -6308,16 +6344,16 @@
         <v>230</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O110" s="1">
         <v>4.99</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.5">
@@ -6325,10 +6361,13 @@
         <v>122</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>235</v>
@@ -6343,16 +6382,16 @@
         <v>230</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O111" s="1">
         <v>17.760000000000002</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.5">
@@ -6360,10 +6399,10 @@
         <v>122</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>236</v>
@@ -6378,16 +6417,16 @@
         <v>230</v>
       </c>
       <c r="M112" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O112" s="1">
         <v>4</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.5">
@@ -6395,10 +6434,10 @@
         <v>122</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>237</v>
@@ -6413,16 +6452,16 @@
         <v>239</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O113" s="1">
         <v>13.12</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.5">
@@ -6430,10 +6469,13 @@
         <v>122</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>240</v>
@@ -6448,16 +6490,16 @@
         <v>239</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O114" s="1">
         <v>27.39</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.5">
@@ -6465,10 +6507,10 @@
         <v>122</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>241</v>
@@ -6483,16 +6525,16 @@
         <v>239</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O115" s="1">
         <v>1</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.5">
@@ -6500,7 +6542,10 @@
         <v>122</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>242</v>
@@ -6518,16 +6563,16 @@
         <v>245</v>
       </c>
       <c r="M116" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O116" s="1">
         <v>13</v>
       </c>
       <c r="P116" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.5">
@@ -6535,7 +6580,7 @@
         <v>122</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>246</v>
@@ -6553,16 +6598,16 @@
         <v>245</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O117" s="1">
         <v>4</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.5">
@@ -6570,13 +6615,13 @@
         <v>122</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>248</v>
@@ -6591,13 +6636,13 @@
         <v>245</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O118" s="1">
         <v>133.41999999999999</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.5">
@@ -6605,10 +6650,10 @@
         <v>122</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>249</v>
@@ -6623,13 +6668,13 @@
         <v>245</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O119" s="1">
         <v>41.05</v>
       </c>
       <c r="P119" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.5">
@@ -6637,34 +6682,34 @@
         <v>250</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J120" s="1">
         <v>2014</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O120" s="1">
         <v>1.17</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.5">
@@ -6672,34 +6717,34 @@
         <v>250</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J121" s="1">
         <v>2014</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O121" s="1">
         <v>0.54</v>
       </c>
       <c r="P121" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.5">
@@ -6707,34 +6752,34 @@
         <v>250</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J122" s="1">
         <v>2014</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O122" s="1">
         <v>-0.06</v>
       </c>
       <c r="P122" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.5">
@@ -6742,34 +6787,34 @@
         <v>250</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>283</v>
+        <v>389</v>
       </c>
       <c r="J123" s="1">
         <v>2014</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O123" s="1">
         <v>0.59</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.5">
@@ -6777,10 +6822,10 @@
         <v>250</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>251</v>
@@ -6795,7 +6840,7 @@
         <v>252</v>
       </c>
       <c r="M124" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="N124" s="1" t="s">
         <v>253</v>
@@ -6804,7 +6849,7 @@
         <v>3</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.5">
@@ -6812,7 +6857,10 @@
         <v>250</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>254</v>
@@ -6830,7 +6878,7 @@
         <v>257</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="N125" s="1" t="s">
         <v>25</v>
@@ -6839,7 +6887,7 @@
         <v>0.43</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.5">
@@ -6847,7 +6895,7 @@
         <v>250</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>258</v>
@@ -6865,7 +6913,7 @@
         <v>257</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="N126" s="1" t="s">
         <v>25</v>
@@ -6874,7 +6922,7 @@
         <v>0.3</v>
       </c>
       <c r="P126" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.5">
@@ -6882,7 +6930,7 @@
         <v>250</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>260</v>
@@ -6900,7 +6948,7 @@
         <v>257</v>
       </c>
       <c r="M127" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="N127" s="1" t="s">
         <v>25</v>
@@ -6909,7 +6957,7 @@
         <v>0.2</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.5">
@@ -6917,7 +6965,10 @@
         <v>250</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>262</v>
@@ -6935,7 +6986,7 @@
         <v>257</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="N128" s="1" t="s">
         <v>25</v>
@@ -6944,7 +6995,7 @@
         <v>0.61</v>
       </c>
       <c r="P128" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.5">
@@ -6952,10 +7003,10 @@
         <v>250</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>264</v>
@@ -6970,7 +7021,7 @@
         <v>257</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="N129" s="1" t="s">
         <v>25</v>
@@ -6979,7 +7030,7 @@
         <v>0.38</v>
       </c>
       <c r="P129" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tract data dict
</commit_message>
<xml_diff>
--- a/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
+++ b/data_final/consolidated/dictionaries/T_Latest_Dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimer\github\opioid-policy-scan\data_final\consolidated\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6081D5F8-269A-4E07-99DA-FC220BB0D6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC73E993-7A36-4220-A024-B9C356220D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22943" yWindow="-14655" windowWidth="38595" windowHeight="21795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="395">
   <si>
     <t>Theme</t>
   </si>
@@ -1203,6 +1203,21 @@
   </si>
   <si>
     <t>Raw Mixed Immigrant Cohesion and Accessibility (MICA) Index (https://sdohatlas.github.io/)</t>
+  </si>
+  <si>
+    <t>Age45_54</t>
+  </si>
+  <si>
+    <t>Total population between 45 and 54 years of age.</t>
+  </si>
+  <si>
+    <t>IPUMS NHGIS</t>
+  </si>
+  <si>
+    <t>Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 1980 Census data does not allow for disaggregation into Age45_49 and Age50_54 variables, so this variable is used instead. </t>
   </si>
 </sst>
 </file>
@@ -2055,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q129"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2722,7 +2737,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -2772,7 +2787,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -2822,7 +2837,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -2858,7 +2873,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2908,7 +2923,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -2955,7 +2970,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -3002,7 +3017,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3049,7 +3064,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3096,7 +3111,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -3143,7 +3158,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -3190,7 +3205,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -3237,7 +3252,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -3281,7 +3296,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -3325,54 +3340,37 @@
         <v>319</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>311</v>
-      </c>
+      <c r="D30" s="3"/>
       <c r="H30" s="1" t="s">
-        <v>67</v>
+        <v>390</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>68</v>
+        <v>391</v>
       </c>
       <c r="J30" s="1">
-        <v>2018</v>
+        <v>1980</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>23</v>
+        <v>392</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="O30" s="1">
-        <v>718</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="Q30" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -3392,10 +3390,10 @@
         <v>311</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J31" s="1">
         <v>2018</v>
@@ -3413,13 +3411,13 @@
         <v>286</v>
       </c>
       <c r="O31" s="1">
-        <v>372</v>
+        <v>718</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -3439,10 +3437,10 @@
         <v>311</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J32" s="1">
         <v>2018</v>
@@ -3460,7 +3458,7 @@
         <v>286</v>
       </c>
       <c r="O32" s="1">
-        <v>1116</v>
+        <v>372</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>319</v>
@@ -3470,7 +3468,15 @@
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="B33" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>311</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>311</v>
       </c>
@@ -3478,10 +3484,10 @@
         <v>311</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J33" s="1">
         <v>2018</v>
@@ -3499,7 +3505,7 @@
         <v>286</v>
       </c>
       <c r="O33" s="1">
-        <v>7468</v>
+        <v>1116</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>319</v>
@@ -3509,29 +3515,18 @@
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>311</v>
-      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="1" t="s">
         <v>311</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H34" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J34" s="1">
         <v>2018</v>
@@ -3549,7 +3544,7 @@
         <v>286</v>
       </c>
       <c r="O34" s="1">
-        <v>6352</v>
+        <v>7468</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>319</v>
@@ -3559,6 +3554,12 @@
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="D35" s="3" t="s">
         <v>311</v>
       </c>
@@ -3572,10 +3573,10 @@
         <v>311</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J35" s="1">
         <v>2018</v>
@@ -3590,24 +3591,18 @@
         <v>366</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O35" s="1">
-        <v>8.9</v>
+        <v>6352</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>311</v>
+        <v>21</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>311</v>
@@ -3622,10 +3617,10 @@
         <v>311</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J36" s="1">
         <v>2018</v>
@@ -3643,15 +3638,24 @@
         <v>287</v>
       </c>
       <c r="O36" s="1">
-        <v>3.78</v>
+        <v>8.9</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>21</v>
+        <v>97</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>311</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>311</v>
@@ -3663,31 +3667,31 @@
         <v>311</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J37" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O37" s="1">
-        <v>15.7</v>
+        <v>3.78</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.5">
@@ -3704,31 +3708,31 @@
         <v>311</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J38" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O38" s="1">
-        <v>4.26</v>
+        <v>15.7</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.5">
@@ -3745,10 +3749,10 @@
         <v>311</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J39" s="1">
         <v>2018</v>
@@ -3766,45 +3770,51 @@
         <v>287</v>
       </c>
       <c r="O39" s="1">
-        <v>18.39</v>
+        <v>4.26</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E40" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="F40" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G40" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J40" s="1">
         <v>2018</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O40" s="1">
-        <v>0</v>
+        <v>18.39</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.5">
@@ -3815,10 +3825,10 @@
         <v>311</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J41" s="1">
         <v>2018</v>
@@ -3850,10 +3860,10 @@
         <v>311</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J42" s="1">
         <v>2018</v>
@@ -3879,49 +3889,37 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>311</v>
+        <v>21</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H43" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="J43" s="1">
         <v>2018</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O43" s="1">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.5">
@@ -3944,10 +3942,10 @@
         <v>311</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J44" s="1">
         <v>2018</v>
@@ -3965,16 +3963,25 @@
         <v>287</v>
       </c>
       <c r="O44" s="1">
-        <v>14.2</v>
+        <v>5.6</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="F45" s="1" t="s">
         <v>311</v>
       </c>
@@ -3982,10 +3989,10 @@
         <v>311</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>309</v>
+        <v>112</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J45" s="1">
         <v>2018</v>
@@ -3996,23 +4003,23 @@
       <c r="L45" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="M45" s="1" t="s">
+        <v>374</v>
+      </c>
       <c r="N45" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O45" s="1">
-        <v>31504</v>
+        <v>14.2</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="F46" s="1" t="s">
         <v>311</v>
       </c>
@@ -4020,10 +4027,10 @@
         <v>311</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>114</v>
+        <v>309</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>310</v>
+        <v>115</v>
       </c>
       <c r="J46" s="1">
         <v>2018</v>
@@ -4034,52 +4041,55 @@
       <c r="L46" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M46" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="N46" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O46" s="1">
-        <v>29969</v>
+        <v>31504</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="D47" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="F47" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G47" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H47" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="J47" s="1">
         <v>2018</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O47" s="1">
-        <v>9.1</v>
+        <v>29969</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.5">
@@ -4090,10 +4100,10 @@
         <v>311</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J48" s="1">
         <v>2018</v>
@@ -4108,13 +4118,13 @@
         <v>375</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O48" s="1">
-        <v>128</v>
+        <v>9.1</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.5">
@@ -4124,32 +4134,32 @@
       <c r="F49" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H49" s="1" t="s">
-        <v>288</v>
+        <v>119</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J49" s="1">
         <v>2018</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>28</v>
+        <v>118</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>375</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O49" s="1">
-        <v>0.38</v>
+        <v>128</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.5">
@@ -4159,11 +4169,14 @@
       <c r="F50" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G50" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H50" s="1" t="s">
-        <v>98</v>
+        <v>288</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="J50" s="1">
         <v>2018</v>
@@ -4174,17 +4187,14 @@
       <c r="L50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M50" s="1" t="s">
-        <v>372</v>
-      </c>
       <c r="N50" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O50" s="1">
-        <v>8.0299999999999994</v>
+        <v>0.38</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.5">
@@ -4194,14 +4204,11 @@
       <c r="F51" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H51" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J51" s="1">
         <v>2018</v>
@@ -4219,7 +4226,7 @@
         <v>287</v>
       </c>
       <c r="O51" s="1">
-        <v>16.18</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>335</v>
@@ -4232,11 +4239,14 @@
       <c r="F52" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G52" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H52" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J52" s="1">
         <v>2018</v>
@@ -4254,7 +4264,7 @@
         <v>287</v>
       </c>
       <c r="O52" s="1">
-        <v>14.7</v>
+        <v>16.18</v>
       </c>
       <c r="P52" s="1" t="s">
         <v>335</v>
@@ -4268,10 +4278,10 @@
         <v>311</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J53" s="1">
         <v>2018</v>
@@ -4289,7 +4299,7 @@
         <v>287</v>
       </c>
       <c r="O53" s="1">
-        <v>15.39</v>
+        <v>14.7</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>335</v>
@@ -4303,10 +4313,10 @@
         <v>311</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J54" s="1">
         <v>2018</v>
@@ -4318,16 +4328,16 @@
         <v>28</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O54" s="1">
-        <v>2092</v>
+        <v>15.39</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.5">
@@ -4337,14 +4347,11 @@
       <c r="F55" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H55" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J55" s="1">
         <v>2018</v>
@@ -4359,18 +4366,18 @@
         <v>373</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O55" s="1">
-        <v>37.65</v>
+        <v>2092</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>311</v>
@@ -4379,49 +4386,37 @@
         <v>311</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="J56" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O56" s="1">
-        <v>6.64</v>
+        <v>37.65</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="F57" s="1" t="s">
         <v>311</v>
       </c>
@@ -4429,45 +4424,60 @@
         <v>311</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J57" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O57" s="1">
-        <v>11.72</v>
+        <v>6.64</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="B58" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="F58" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G58" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H58" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J58" s="1">
         <v>2018</v>
@@ -4485,7 +4495,7 @@
         <v>287</v>
       </c>
       <c r="O58" s="1">
-        <v>0.68</v>
+        <v>11.72</v>
       </c>
       <c r="P58" s="1" t="s">
         <v>337</v>
@@ -4499,10 +4509,10 @@
         <v>311</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J59" s="1">
         <v>2018</v>
@@ -4520,10 +4530,10 @@
         <v>287</v>
       </c>
       <c r="O59" s="1">
-        <v>8.66</v>
+        <v>0.68</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.5">
@@ -4534,10 +4544,10 @@
         <v>311</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J60" s="1">
         <v>2018</v>
@@ -4555,7 +4565,7 @@
         <v>287</v>
       </c>
       <c r="O60" s="1">
-        <v>19.899999999999999</v>
+        <v>8.66</v>
       </c>
       <c r="P60" s="1" t="s">
         <v>338</v>
@@ -4569,10 +4579,10 @@
         <v>311</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J61" s="1">
         <v>2018</v>
@@ -4590,10 +4600,10 @@
         <v>287</v>
       </c>
       <c r="O61" s="1">
-        <v>673.09</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.5">
@@ -4604,31 +4614,31 @@
         <v>311</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J62" s="1">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>139</v>
+        <v>23</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>253</v>
+        <v>287</v>
       </c>
       <c r="O62" s="1">
-        <v>1</v>
+        <v>673.09</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.5">
@@ -4639,10 +4649,10 @@
         <v>311</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J63" s="1">
         <v>2010</v>
@@ -4660,7 +4670,7 @@
         <v>253</v>
       </c>
       <c r="O63" s="1">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="P63" s="1" t="s">
         <v>339</v>
@@ -4673,14 +4683,11 @@
       <c r="F64" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G64" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H64" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J64" s="1">
         <v>2010</v>
@@ -4695,10 +4702,10 @@
         <v>378</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="O64" s="1" t="s">
-        <v>305</v>
+        <v>253</v>
+      </c>
+      <c r="O64" s="1">
+        <v>1.1000000000000001</v>
       </c>
       <c r="P64" s="1" t="s">
         <v>339</v>
@@ -4706,51 +4713,54 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G65" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H65" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J65" s="1">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="O65" s="1">
-        <v>6.73</v>
+        <v>289</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>311</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J66" s="1">
         <v>2018</v>
@@ -4765,13 +4775,13 @@
         <v>379</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O66" s="1">
-        <v>1</v>
+        <v>6.73</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.5">
@@ -4782,10 +4792,10 @@
         <v>311</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J67" s="1">
         <v>2018</v>
@@ -4800,10 +4810,10 @@
         <v>379</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O67" s="1">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="P67" s="1" t="s">
         <v>340</v>
@@ -4817,10 +4827,10 @@
         <v>311</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J68" s="1">
         <v>2018</v>
@@ -4838,7 +4848,7 @@
         <v>287</v>
       </c>
       <c r="O68" s="1">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="P68" s="1" t="s">
         <v>340</v>
@@ -4851,35 +4861,32 @@
       <c r="F69" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G69" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H69" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>304</v>
+        <v>154</v>
       </c>
       <c r="J69" s="1">
         <v>2018</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O69" s="1">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.5">
@@ -4889,32 +4896,35 @@
       <c r="F70" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G70" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H70" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>159</v>
+        <v>304</v>
       </c>
       <c r="J70" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O70" s="1">
-        <v>0.81</v>
+        <v>0.15</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.5">
@@ -4925,10 +4935,10 @@
         <v>311</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J71" s="1">
         <v>2019</v>
@@ -4959,14 +4969,11 @@
       <c r="F72" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G72" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H72" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J72" s="1">
         <v>2019</v>
@@ -4984,10 +4991,10 @@
         <v>287</v>
       </c>
       <c r="O72" s="1">
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.5">
@@ -4997,11 +5004,14 @@
       <c r="F73" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G73" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H73" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J73" s="1">
         <v>2019</v>
@@ -5016,13 +5026,13 @@
         <v>381</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O73" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>319</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.5">
@@ -5033,10 +5043,10 @@
         <v>311</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J74" s="1">
         <v>2019</v>
@@ -5051,13 +5061,13 @@
         <v>381</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O74" s="1">
-        <v>13.22</v>
+        <v>21</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.5">
@@ -5067,14 +5077,11 @@
       <c r="F75" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G75" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H75" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J75" s="1">
         <v>2019</v>
@@ -5092,10 +5099,10 @@
         <v>287</v>
       </c>
       <c r="O75" s="1">
-        <v>27.39</v>
+        <v>13.22</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.5">
@@ -5105,11 +5112,14 @@
       <c r="F76" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G76" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H76" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="J76" s="1">
         <v>2019</v>
@@ -5124,13 +5134,13 @@
         <v>381</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O76" s="1">
-        <v>1</v>
+        <v>27.39</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.5">
@@ -5141,10 +5151,10 @@
         <v>311</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="J77" s="1">
         <v>2019</v>
@@ -5159,13 +5169,13 @@
         <v>381</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O77" s="1">
-        <v>18.04</v>
+        <v>1</v>
       </c>
       <c r="P77" s="1" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.5">
@@ -5175,14 +5185,11 @@
       <c r="F78" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H78" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J78" s="1">
         <v>2019</v>
@@ -5200,10 +5207,10 @@
         <v>287</v>
       </c>
       <c r="O78" s="1">
-        <v>35.340000000000003</v>
+        <v>18.04</v>
       </c>
       <c r="P78" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.5">
@@ -5213,11 +5220,14 @@
       <c r="F79" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G79" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H79" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J79" s="1">
         <v>2019</v>
@@ -5232,30 +5242,27 @@
         <v>381</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O79" s="1">
-        <v>0</v>
+        <v>35.340000000000003</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>122</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G80" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H80" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>313</v>
+        <v>178</v>
       </c>
       <c r="J80" s="1">
         <v>2019</v>
@@ -5270,27 +5277,30 @@
         <v>381</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O80" s="1">
         <v>0</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.5">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G81" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H81" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>181</v>
+        <v>313</v>
       </c>
       <c r="J81" s="1">
         <v>2019</v>
@@ -5305,13 +5315,13 @@
         <v>381</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O81" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.5">
@@ -5322,10 +5332,10 @@
         <v>311</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J82" s="1">
         <v>2019</v>
@@ -5356,14 +5366,11 @@
       <c r="F83" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G83" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H83" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>314</v>
+        <v>183</v>
       </c>
       <c r="J83" s="1">
         <v>2019</v>
@@ -5378,13 +5385,13 @@
         <v>381</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O83" s="1">
-        <v>1744.66</v>
+        <v>2</v>
       </c>
       <c r="P83" s="1" t="s">
-        <v>347</v>
+        <v>319</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.5">
@@ -5394,11 +5401,14 @@
       <c r="F84" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G84" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H84" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>186</v>
+        <v>314</v>
       </c>
       <c r="J84" s="1">
         <v>2019</v>
@@ -5413,13 +5423,13 @@
         <v>381</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O84" s="1">
-        <v>0</v>
+        <v>1744.66</v>
       </c>
       <c r="P84" s="1" t="s">
-        <v>319</v>
+        <v>347</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.5">
@@ -5430,10 +5440,10 @@
         <v>311</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J85" s="1">
         <v>2019</v>
@@ -5464,14 +5474,11 @@
       <c r="F86" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G86" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H86" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>315</v>
+        <v>188</v>
       </c>
       <c r="J86" s="1">
         <v>2019</v>
@@ -5486,13 +5493,13 @@
         <v>381</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="O86" s="1" t="s">
-        <v>316</v>
+        <v>286</v>
+      </c>
+      <c r="O86" s="1">
+        <v>0</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.5">
@@ -5502,11 +5509,14 @@
       <c r="F87" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G87" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H87" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>191</v>
+        <v>315</v>
       </c>
       <c r="J87" s="1">
         <v>2019</v>
@@ -5521,13 +5531,13 @@
         <v>381</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="O87" s="1">
-        <v>0</v>
+        <v>287</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="P87" s="1" t="s">
-        <v>319</v>
+        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.5">
@@ -5538,10 +5548,10 @@
         <v>311</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J88" s="1">
         <v>2019</v>
@@ -5572,14 +5582,11 @@
       <c r="F89" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G89" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H89" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J89" s="1">
         <v>2019</v>
@@ -5594,13 +5601,13 @@
         <v>381</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O89" s="1">
         <v>0</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>349</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.5">
@@ -5610,11 +5617,14 @@
       <c r="F90" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G90" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H90" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J90" s="1">
         <v>2019</v>
@@ -5629,13 +5639,13 @@
         <v>381</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O90" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P90" s="1" t="s">
-        <v>319</v>
+        <v>349</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.5">
@@ -5646,10 +5656,10 @@
         <v>311</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J91" s="1">
         <v>2019</v>
@@ -5667,7 +5677,7 @@
         <v>286</v>
       </c>
       <c r="O91" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P91" s="1" t="s">
         <v>319</v>
@@ -5680,14 +5690,11 @@
       <c r="F92" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G92" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H92" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J92" s="1">
         <v>2019</v>
@@ -5702,13 +5709,13 @@
         <v>381</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O92" s="1">
-        <v>148.18</v>
+        <v>3</v>
       </c>
       <c r="P92" s="1" t="s">
-        <v>350</v>
+        <v>319</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.5">
@@ -5718,11 +5725,14 @@
       <c r="F93" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G93" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H93" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J93" s="1">
         <v>2019</v>
@@ -5737,13 +5747,13 @@
         <v>381</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O93" s="1">
-        <v>0</v>
+        <v>148.18</v>
       </c>
       <c r="P93" s="1" t="s">
-        <v>319</v>
+        <v>350</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.5">
@@ -5754,10 +5764,10 @@
         <v>311</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J94" s="1">
         <v>2019</v>
@@ -5788,14 +5798,11 @@
       <c r="F95" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H95" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J95" s="1">
         <v>2019</v>
@@ -5810,13 +5817,13 @@
         <v>381</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O95" s="1">
-        <v>165.18</v>
+        <v>0</v>
       </c>
       <c r="P95" s="1" t="s">
-        <v>351</v>
+        <v>319</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.5">
@@ -5826,11 +5833,14 @@
       <c r="F96" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G96" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H96" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J96" s="1">
         <v>2019</v>
@@ -5845,13 +5855,13 @@
         <v>381</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O96" s="1">
-        <v>0</v>
+        <v>165.18</v>
       </c>
       <c r="P96" s="1" t="s">
-        <v>319</v>
+        <v>351</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.5">
@@ -5862,10 +5872,10 @@
         <v>311</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J97" s="1">
         <v>2019</v>
@@ -5897,28 +5907,28 @@
         <v>311</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J98" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>214</v>
+        <v>160</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>215</v>
+        <v>161</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O98" s="1">
-        <v>10.23</v>
+        <v>0</v>
       </c>
       <c r="P98" s="1" t="s">
         <v>319</v>
@@ -5931,14 +5941,11 @@
       <c r="F99" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G99" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H99" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J99" s="1">
         <v>2020</v>
@@ -5956,10 +5963,10 @@
         <v>287</v>
       </c>
       <c r="O99" s="1">
-        <v>19.16</v>
+        <v>10.23</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>352</v>
+        <v>319</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.5">
@@ -5969,11 +5976,14 @@
       <c r="F100" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G100" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H100" s="1" t="s">
-        <v>299</v>
+        <v>216</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J100" s="1">
         <v>2020</v>
@@ -5988,13 +5998,13 @@
         <v>382</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O100" s="1">
-        <v>17</v>
+        <v>19.16</v>
       </c>
       <c r="P100" s="1" t="s">
-        <v>319</v>
+        <v>352</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.5">
@@ -6005,28 +6015,28 @@
         <v>311</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J101" s="1">
         <v>2020</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O101" s="1">
-        <v>0.31</v>
+        <v>17</v>
       </c>
       <c r="P101" s="1" t="s">
         <v>319</v>
@@ -6039,14 +6049,11 @@
       <c r="F102" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G102" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H102" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J102" s="1">
         <v>2020</v>
@@ -6064,10 +6071,10 @@
         <v>287</v>
       </c>
       <c r="O102" s="1">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>353</v>
+        <v>319</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.5">
@@ -6077,11 +6084,14 @@
       <c r="F103" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G103" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H103" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J103" s="1">
         <v>2020</v>
@@ -6096,13 +6106,13 @@
         <v>383</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O103" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>319</v>
+        <v>353</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.5">
@@ -6113,28 +6123,28 @@
         <v>311</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J104" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="L104" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O104" s="1">
-        <v>0.84</v>
+        <v>6</v>
       </c>
       <c r="P104" s="1" t="s">
         <v>319</v>
@@ -6147,14 +6157,11 @@
       <c r="F105" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G105" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H105" s="1" t="s">
-        <v>225</v>
+        <v>290</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J105" s="1">
         <v>2019</v>
@@ -6172,10 +6179,10 @@
         <v>287</v>
       </c>
       <c r="O105" s="1">
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.5">
@@ -6185,11 +6192,14 @@
       <c r="F106" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G106" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H106" s="1" t="s">
-        <v>291</v>
+        <v>225</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J106" s="1">
         <v>2019</v>
@@ -6204,13 +6214,13 @@
         <v>384</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O106" s="1">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>319</v>
+        <v>354</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.5">
@@ -6221,28 +6231,28 @@
         <v>311</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J107" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="L107" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O107" s="1">
-        <v>0.2</v>
+        <v>58</v>
       </c>
       <c r="P107" s="1" t="s">
         <v>319</v>
@@ -6255,14 +6265,11 @@
       <c r="F108" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G108" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H108" s="1" t="s">
-        <v>231</v>
+        <v>292</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J108" s="1">
         <v>2020</v>
@@ -6280,10 +6287,10 @@
         <v>287</v>
       </c>
       <c r="O108" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.5">
@@ -6293,11 +6300,14 @@
       <c r="F109" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G109" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H109" s="1" t="s">
-        <v>293</v>
+        <v>231</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J109" s="1">
         <v>2020</v>
@@ -6312,13 +6322,13 @@
         <v>385</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O109" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>319</v>
+        <v>355</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.5">
@@ -6329,10 +6339,10 @@
         <v>311</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J110" s="1">
         <v>2020</v>
@@ -6344,16 +6354,16 @@
         <v>230</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O110" s="1">
-        <v>4.99</v>
+        <v>3</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.5">
@@ -6363,14 +6373,11 @@
       <c r="F111" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G111" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H111" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J111" s="1">
         <v>2020</v>
@@ -6388,10 +6395,10 @@
         <v>287</v>
       </c>
       <c r="O111" s="1">
-        <v>17.760000000000002</v>
+        <v>4.99</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.5">
@@ -6401,11 +6408,14 @@
       <c r="F112" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G112" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H112" s="1" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J112" s="1">
         <v>2020</v>
@@ -6420,13 +6430,13 @@
         <v>386</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O112" s="1">
-        <v>4</v>
+        <v>17.760000000000002</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>319</v>
+        <v>356</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.5">
@@ -6437,28 +6447,28 @@
         <v>311</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J113" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O113" s="1">
-        <v>13.12</v>
+        <v>4</v>
       </c>
       <c r="P113" s="1" t="s">
         <v>319</v>
@@ -6471,14 +6481,11 @@
       <c r="F114" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G114" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H114" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J114" s="1">
         <v>2021</v>
@@ -6496,10 +6503,10 @@
         <v>287</v>
       </c>
       <c r="O114" s="1">
-        <v>27.39</v>
+        <v>13.12</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.5">
@@ -6509,11 +6516,14 @@
       <c r="F115" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G115" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H115" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J115" s="1">
         <v>2021</v>
@@ -6528,13 +6538,13 @@
         <v>387</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O115" s="1">
-        <v>1</v>
+        <v>27.39</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>319</v>
+        <v>357</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.5">
@@ -6544,35 +6554,32 @@
       <c r="F116" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G116" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H116" s="1" t="s">
-        <v>242</v>
+        <v>298</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J116" s="1">
-        <v>2010</v>
+        <v>2021</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="M116" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N116" s="1" t="s">
         <v>286</v>
       </c>
       <c r="O116" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="P116" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.5">
@@ -6582,11 +6589,14 @@
       <c r="F117" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G117" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H117" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="J117" s="1">
         <v>2010</v>
@@ -6604,7 +6614,7 @@
         <v>286</v>
       </c>
       <c r="O117" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="P117" s="1" t="s">
         <v>339</v>
@@ -6617,14 +6627,11 @@
       <c r="F118" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G118" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H118" s="1" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J118" s="1">
         <v>2010</v>
@@ -6635,14 +6642,17 @@
       <c r="L118" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="M118" s="1" t="s">
+        <v>388</v>
+      </c>
       <c r="N118" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O118" s="1">
-        <v>133.41999999999999</v>
+        <v>4</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.5">
@@ -6652,11 +6662,14 @@
       <c r="F119" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G119" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H119" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J119" s="1">
         <v>2010</v>
@@ -6671,45 +6684,42 @@
         <v>287</v>
       </c>
       <c r="O119" s="1">
-        <v>41.05</v>
+        <v>133.41999999999999</v>
       </c>
       <c r="P119" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
-        <v>250</v>
+        <v>122</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G120" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H120" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
       <c r="J120" s="1">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>283</v>
+        <v>244</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="N120" s="1" t="s">
         <v>287</v>
       </c>
       <c r="O120" s="1">
-        <v>1.17</v>
+        <v>41.05</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.5">
@@ -6723,10 +6733,10 @@
         <v>311</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J121" s="1">
         <v>2014</v>
@@ -6741,7 +6751,7 @@
         <v>287</v>
       </c>
       <c r="O121" s="1">
-        <v>0.54</v>
+        <v>1.17</v>
       </c>
       <c r="P121" s="1" t="s">
         <v>341</v>
@@ -6758,10 +6768,10 @@
         <v>311</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J122" s="1">
         <v>2014</v>
@@ -6776,7 +6786,7 @@
         <v>287</v>
       </c>
       <c r="O122" s="1">
-        <v>-0.06</v>
+        <v>0.54</v>
       </c>
       <c r="P122" s="1" t="s">
         <v>341</v>
@@ -6793,10 +6803,10 @@
         <v>311</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>389</v>
+        <v>281</v>
       </c>
       <c r="J123" s="1">
         <v>2014</v>
@@ -6811,7 +6821,7 @@
         <v>287</v>
       </c>
       <c r="O123" s="1">
-        <v>0.59</v>
+        <v>-0.06</v>
       </c>
       <c r="P123" s="1" t="s">
         <v>341</v>
@@ -6824,32 +6834,32 @@
       <c r="F124" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G124" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H124" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>251</v>
+        <v>389</v>
       </c>
       <c r="J124" s="1">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>252</v>
+        <v>283</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="M124" s="1" t="s">
-        <v>367</v>
+        <v>282</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>253</v>
+        <v>287</v>
       </c>
       <c r="O124" s="1">
-        <v>3</v>
+        <v>0.59</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.5">
@@ -6859,35 +6869,32 @@
       <c r="F125" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G125" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H125" s="1" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J125" s="1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>25</v>
+        <v>253</v>
       </c>
       <c r="O125" s="1">
-        <v>0.43</v>
+        <v>3</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.5">
@@ -6897,11 +6904,14 @@
       <c r="F126" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G126" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H126" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J126" s="1">
         <v>2018</v>
@@ -6919,10 +6929,10 @@
         <v>25</v>
       </c>
       <c r="O126" s="1">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
       <c r="P126" s="1" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.5">
@@ -6933,10 +6943,10 @@
         <v>311</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J127" s="1">
         <v>2018</v>
@@ -6954,10 +6964,10 @@
         <v>25</v>
       </c>
       <c r="O127" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.5">
@@ -6967,14 +6977,11 @@
       <c r="F128" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G128" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="H128" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J128" s="1">
         <v>2018</v>
@@ -6992,10 +6999,10 @@
         <v>25</v>
       </c>
       <c r="O128" s="1">
-        <v>0.61</v>
+        <v>0.2</v>
       </c>
       <c r="P128" s="1" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.5">
@@ -7005,11 +7012,14 @@
       <c r="F129" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G129" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H129" s="1" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J129" s="1">
         <v>2018</v>
@@ -7027,9 +7037,44 @@
         <v>25</v>
       </c>
       <c r="O129" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A130" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J130" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="N130" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O130" s="1">
         <v>0.38</v>
       </c>
-      <c r="P129" s="1" t="s">
+      <c r="P130" s="1" t="s">
         <v>362</v>
       </c>
     </row>

</xml_diff>